<commit_message>
that was a long way
</commit_message>
<xml_diff>
--- a/Setup.xlsx
+++ b/Setup.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eliad\Desktop\Edu\WU Wien\Thesis\Master-Thesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86D73A8E-8EC4-43A6-A520-A1DEB05E8E66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D65DC436-9B83-4A44-B0E8-C05806DE0DB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{DFD7175C-8BF9-4F5D-BF57-2014F8D04D64}"/>
+    <workbookView xWindow="28680" yWindow="4485" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{DFD7175C-8BF9-4F5D-BF57-2014F8D04D64}"/>
   </bookViews>
   <sheets>
     <sheet name="Countries" sheetId="2" r:id="rId1"/>
@@ -40,17 +40,27 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
+    <author>tc={7D8E0F55-43F1-41CB-8406-B15EDBF37B95}</author>
     <author>tc={B7E71C5C-C4F8-4A7D-A23A-4249918D874D}</author>
     <author>tc={A440696A-8FBF-44CB-ACA8-73A2B1BE2A85}</author>
     <author>tc={1BF648E4-22D4-45B6-9EBB-F0CD4471AD7C}</author>
     <author>tc={F2A473D3-543D-45B8-AF20-81FF2D86C488}</author>
+    <author>tc={BBCC0A15-7BD6-4921-9CD2-9330C5D45A5F}</author>
     <author>tc={5016BFA2-34DF-4282-9BE8-C6F627D2AE3E}</author>
     <author>tc={EE5A5CAE-7AFD-47A5-A294-920C6BE72CEF}</author>
     <author>tc={5ACF80A4-3273-4F9E-8727-538787B277A3}</author>
     <author>tc={61876B84-F5DA-451B-998D-6C7D7286518F}</author>
   </authors>
   <commentList>
-    <comment ref="E16" authorId="0" shapeId="0" xr:uid="{B7E71C5C-C4F8-4A7D-A23A-4249918D874D}">
+    <comment ref="A16" authorId="0" shapeId="0" xr:uid="{7D8E0F55-43F1-41CB-8406-B15EDBF37B95}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Also available in eurostat under economically active population</t>
+      </text>
+    </comment>
+    <comment ref="E16" authorId="1" shapeId="0" xr:uid="{B7E71C5C-C4F8-4A7D-A23A-4249918D874D}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -58,7 +68,7 @@
     Also available in 1000 in Ardeco</t>
       </text>
     </comment>
-    <comment ref="J24" authorId="1" shapeId="0" xr:uid="{A440696A-8FBF-44CB-ACA8-73A2B1BE2A85}">
+    <comment ref="J24" authorId="2" shapeId="0" xr:uid="{A440696A-8FBF-44CB-ACA8-73A2B1BE2A85}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -66,7 +76,7 @@
     Net Wage is from 2011 onwards</t>
       </text>
     </comment>
-    <comment ref="A41" authorId="2" shapeId="0" xr:uid="{1BF648E4-22D4-45B6-9EBB-F0CD4471AD7C}">
+    <comment ref="A39" authorId="3" shapeId="0" xr:uid="{1BF648E4-22D4-45B6-9EBB-F0CD4471AD7C}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -74,7 +84,7 @@
     Homicide/robbery/burglary/theft (the last 2 consistent from 2012)</t>
       </text>
     </comment>
-    <comment ref="E41" authorId="3" shapeId="0" xr:uid="{F2A473D3-543D-45B8-AF20-81FF2D86C488}">
+    <comment ref="E39" authorId="4" shapeId="0" xr:uid="{F2A473D3-543D-45B8-AF20-81FF2D86C488}">
       <text>
         <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -83,7 +93,15 @@
 </t>
       </text>
     </comment>
-    <comment ref="F49" authorId="4" shapeId="0" xr:uid="{5016BFA2-34DF-4282-9BE8-C6F627D2AE3E}">
+    <comment ref="J39" authorId="5" shapeId="0" xr:uid="{BBCC0A15-7BD6-4921-9CD2-9330C5D45A5F}">
+      <text>
+        <t xml:space="preserve">[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Recorded crimes by Districts/Regions, Type of crime and Years. PxWeb (statistica.md) </t>
+      </text>
+    </comment>
+    <comment ref="F47" authorId="6" shapeId="0" xr:uid="{5016BFA2-34DF-4282-9BE8-C6F627D2AE3E}">
       <text>
         <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -92,7 +110,7 @@
 </t>
       </text>
     </comment>
-    <comment ref="E51" authorId="5" shapeId="0" xr:uid="{EE5A5CAE-7AFD-47A5-A294-920C6BE72CEF}">
+    <comment ref="E49" authorId="7" shapeId="0" xr:uid="{EE5A5CAE-7AFD-47A5-A294-920C6BE72CEF}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -100,7 +118,7 @@
     Not nace but other classification let seee</t>
       </text>
     </comment>
-    <comment ref="F51" authorId="6" shapeId="0" xr:uid="{5ACF80A4-3273-4F9E-8727-538787B277A3}">
+    <comment ref="F49" authorId="8" shapeId="0" xr:uid="{5ACF80A4-3273-4F9E-8727-538787B277A3}">
       <text>
         <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -108,7 +126,7 @@
     Publications | Statistical Office of the Republic of Serbia </t>
       </text>
     </comment>
-    <comment ref="F53" authorId="7" shapeId="0" xr:uid="{61876B84-F5DA-451B-998D-6C7D7286518F}">
+    <comment ref="F51" authorId="9" shapeId="0" xr:uid="{61876B84-F5DA-451B-998D-6C7D7286518F}">
       <text>
         <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -121,7 +139,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="573" uniqueCount="292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="595" uniqueCount="290">
   <si>
     <t>Macedonia</t>
   </si>
@@ -684,12 +702,6 @@
     <t>Employement in high technology sectors</t>
   </si>
   <si>
-    <t>Economically active population</t>
-  </si>
-  <si>
-    <t>Economic activity rate</t>
-  </si>
-  <si>
     <t>Employement by edu</t>
   </si>
   <si>
@@ -957,9 +969,6 @@
     <t>2011/2013</t>
   </si>
   <si>
-    <t>age alternatives</t>
-  </si>
-  <si>
     <t>Interruction in time series for MK ME RS</t>
   </si>
   <si>
@@ -997,6 +1006,9 @@
   </si>
   <si>
     <t>☺</t>
+  </si>
+  <si>
+    <t>Nato Membership</t>
   </si>
 </sst>
 </file>
@@ -1410,7 +1422,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1444,9 +1456,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1484,7 +1496,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1590,7 +1602,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1732,7 +1744,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1740,16 +1752,19 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="A16" dT="2024-05-11T06:57:34.28" personId="{D4968EC9-A480-41EA-BA73-9962D579C6C6}" id="{7D8E0F55-43F1-41CB-8406-B15EDBF37B95}">
+    <text>Also available in eurostat under economically active population</text>
+  </threadedComment>
   <threadedComment ref="E16" dT="2024-04-20T21:28:37.96" personId="{D4968EC9-A480-41EA-BA73-9962D579C6C6}" id="{B7E71C5C-C4F8-4A7D-A23A-4249918D874D}">
     <text>Also available in 1000 in Ardeco</text>
   </threadedComment>
   <threadedComment ref="J24" dT="2024-04-19T20:00:47.45" personId="{D4968EC9-A480-41EA-BA73-9962D579C6C6}" id="{A440696A-8FBF-44CB-ACA8-73A2B1BE2A85}">
     <text>Net Wage is from 2011 onwards</text>
   </threadedComment>
-  <threadedComment ref="A41" dT="2024-04-20T20:20:13.06" personId="{D4968EC9-A480-41EA-BA73-9962D579C6C6}" id="{1BF648E4-22D4-45B6-9EBB-F0CD4471AD7C}">
+  <threadedComment ref="A39" dT="2024-04-20T20:20:13.06" personId="{D4968EC9-A480-41EA-BA73-9962D579C6C6}" id="{1BF648E4-22D4-45B6-9EBB-F0CD4471AD7C}">
     <text>Homicide/robbery/burglary/theft (the last 2 consistent from 2012)</text>
   </threadedComment>
-  <threadedComment ref="E41" dT="2024-04-28T09:22:40.49" personId="{D4968EC9-A480-41EA-BA73-9962D579C6C6}" id="{F2A473D3-543D-45B8-AF20-81FF2D86C488}">
+  <threadedComment ref="E39" dT="2024-04-28T09:22:40.49" personId="{D4968EC9-A480-41EA-BA73-9962D579C6C6}" id="{F2A473D3-543D-45B8-AF20-81FF2D86C488}">
     <text xml:space="preserve">Under Judicature if needed: PxWeb - Select table (stat.gov.mk) 
 </text>
     <extLst>
@@ -1759,14 +1774,23 @@
       </x:ext>
     </extLst>
   </threadedComment>
-  <threadedComment ref="F49" dT="2024-04-27T17:35:46.47" personId="{D4968EC9-A480-41EA-BA73-9962D579C6C6}" id="{5016BFA2-34DF-4282-9BE8-C6F627D2AE3E}">
+  <threadedComment ref="J39" dT="2024-05-11T07:43:35.38" personId="{D4968EC9-A480-41EA-BA73-9962D579C6C6}" id="{BBCC0A15-7BD6-4921-9CD2-9330C5D45A5F}">
+    <text xml:space="preserve">Recorded crimes by Districts/Regions, Type of crime and Years. PxWeb (statistica.md) </text>
+    <extLst>
+      <x:ext xmlns:xltc2="http://schemas.microsoft.com/office/spreadsheetml/2020/threadedcomments2" uri="{F7C98A9C-CBB3-438F-8F68-D28B6AF4A901}">
+        <xltc2:checksum>2655068630</xltc2:checksum>
+        <xltc2:hyperlink startIndex="0" length="84" url="https://statbank.statistica.md/PxWeb/pxweb/en/30%20Statistica%20sociala/30%20Statistica%20sociala__12%20JUS__JUS010/JUS010300reg.px/?rxid=b2ff27d7-0b96-43c9-934b-42e1a2a9a774"/>
+      </x:ext>
+    </extLst>
+  </threadedComment>
+  <threadedComment ref="F47" dT="2024-04-27T17:35:46.47" personId="{D4968EC9-A480-41EA-BA73-9962D579C6C6}" id="{5016BFA2-34DF-4282-9BE8-C6F627D2AE3E}">
     <text xml:space="preserve">Look up on national bank
 </text>
   </threadedComment>
-  <threadedComment ref="E51" dT="2024-04-27T17:03:05.70" personId="{D4968EC9-A480-41EA-BA73-9962D579C6C6}" id="{EE5A5CAE-7AFD-47A5-A294-920C6BE72CEF}">
+  <threadedComment ref="E49" dT="2024-04-27T17:03:05.70" personId="{D4968EC9-A480-41EA-BA73-9962D579C6C6}" id="{EE5A5CAE-7AFD-47A5-A294-920C6BE72CEF}">
     <text>Not nace but other classification let seee</text>
   </threadedComment>
-  <threadedComment ref="F51" dT="2024-04-28T08:54:34.37" personId="{D4968EC9-A480-41EA-BA73-9962D579C6C6}" id="{5ACF80A4-3273-4F9E-8727-538787B277A3}">
+  <threadedComment ref="F49" dT="2024-04-28T08:54:34.37" personId="{D4968EC9-A480-41EA-BA73-9962D579C6C6}" id="{5ACF80A4-3273-4F9E-8727-538787B277A3}">
     <text xml:space="preserve">Publications | Statistical Office of the Republic of Serbia </text>
     <extLst>
       <x:ext xmlns:xltc2="http://schemas.microsoft.com/office/spreadsheetml/2020/threadedcomments2" uri="{F7C98A9C-CBB3-438F-8F68-D28B6AF4A901}">
@@ -1775,7 +1799,7 @@
       </x:ext>
     </extLst>
   </threadedComment>
-  <threadedComment ref="F53" dT="2024-04-28T08:56:24.22" personId="{D4968EC9-A480-41EA-BA73-9962D579C6C6}" id="{61876B84-F5DA-451B-998D-6C7D7286518F}">
+  <threadedComment ref="F51" dT="2024-04-28T08:56:24.22" personId="{D4968EC9-A480-41EA-BA73-9962D579C6C6}" id="{61876B84-F5DA-451B-998D-6C7D7286518F}">
     <text xml:space="preserve">Publications | Statistical Office of the Republic of Serbia </text>
     <extLst>
       <x:ext xmlns:xltc2="http://schemas.microsoft.com/office/spreadsheetml/2020/threadedcomments2" uri="{F7C98A9C-CBB3-438F-8F68-D28B6AF4A901}">
@@ -2550,11 +2574,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E19BF3E-7EEF-423C-8D22-BB79E99E3E18}">
-  <dimension ref="A1:P1803"/>
+  <dimension ref="A1:P1802"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A25" sqref="A25:XFD25"/>
+      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2582,10 +2606,10 @@
         <v>169</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>1</v>
@@ -2600,7 +2624,7 @@
         <v>7</v>
       </c>
       <c r="H1" s="22" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="I1" s="3" t="s">
         <v>4</v>
@@ -2618,38 +2642,40 @@
         <v>8</v>
       </c>
       <c r="N1" s="29" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="2" spans="1:16" s="12" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B2" s="38" t="s">
-        <v>206</v>
-      </c>
-      <c r="C2" s="46"/>
+        <v>204</v>
+      </c>
+      <c r="C2" s="38" t="s">
+        <v>204</v>
+      </c>
       <c r="D2" s="38" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="E2" s="38" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="F2" s="38" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="G2" s="38" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="H2" s="41"/>
       <c r="I2" s="42" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="J2" s="43" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="K2" s="43" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="L2" s="44"/>
       <c r="M2" s="44"/>
@@ -2657,105 +2683,111 @@
     </row>
     <row r="3" spans="1:16" s="12" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B3" s="38" t="s">
-        <v>206</v>
-      </c>
-      <c r="C3" s="46"/>
+        <v>204</v>
+      </c>
+      <c r="C3" s="38" t="s">
+        <v>204</v>
+      </c>
       <c r="D3" s="38" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="E3" s="38" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="F3" s="38" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="G3" s="38" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="H3" s="41"/>
       <c r="I3" s="42" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="J3" s="43" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="K3" s="43" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="L3" s="44"/>
       <c r="M3" s="44"/>
       <c r="N3" s="32" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="4" spans="1:16" s="12" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="21" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B4" s="38" t="s">
-        <v>206</v>
-      </c>
-      <c r="C4" s="46"/>
+        <v>204</v>
+      </c>
+      <c r="C4" s="38" t="s">
+        <v>204</v>
+      </c>
       <c r="D4" s="39" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="E4" s="38" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="F4" s="38" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="G4" s="38" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="H4" s="41"/>
       <c r="I4" s="42" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="J4" s="43" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="K4" s="42" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="L4" s="44"/>
       <c r="M4" s="44"/>
       <c r="N4" s="32" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="5" spans="1:16" s="12" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="21" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B5" s="38" t="s">
-        <v>206</v>
-      </c>
-      <c r="C5" s="46"/>
+        <v>204</v>
+      </c>
+      <c r="C5" s="38" t="s">
+        <v>204</v>
+      </c>
       <c r="D5" s="39" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="E5" s="38" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="F5" s="38" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="G5" s="38" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="H5" s="41"/>
       <c r="I5" s="42" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="J5" s="43" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="K5" s="42" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="L5" s="44"/>
       <c r="M5" s="44"/>
@@ -2766,33 +2798,35 @@
     </row>
     <row r="6" spans="1:16" s="12" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="21" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B6" s="38" t="s">
-        <v>206</v>
-      </c>
-      <c r="C6" s="46"/>
+        <v>204</v>
+      </c>
+      <c r="C6" s="38" t="s">
+        <v>204</v>
+      </c>
       <c r="D6" s="39" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="E6" s="38" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="F6" s="38" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="G6" s="38" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="H6" s="41"/>
       <c r="I6" s="45" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="J6" s="43" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="K6" s="42" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="L6" s="44"/>
       <c r="M6" s="44"/>
@@ -2803,44 +2837,46 @@
     </row>
     <row r="7" spans="1:16" s="12" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="21" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B7" s="38" t="s">
-        <v>206</v>
-      </c>
-      <c r="C7" s="46"/>
+        <v>204</v>
+      </c>
+      <c r="C7" s="38" t="s">
+        <v>204</v>
+      </c>
       <c r="D7" s="39" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="E7" s="38" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="F7" s="38" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="G7" s="38" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="H7" s="41"/>
       <c r="I7" s="45" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="J7" s="43" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="K7" s="42" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="L7" s="44"/>
       <c r="M7" s="44"/>
       <c r="N7" s="29"/>
       <c r="P7" s="19" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
     </row>
     <row r="8" spans="1:16" s="12" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="26" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="B8" s="63"/>
       <c r="C8" s="63"/>
@@ -2849,7 +2885,7 @@
       <c r="F8" s="63"/>
       <c r="G8" s="63"/>
       <c r="H8" s="41" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="I8" s="65"/>
       <c r="J8" s="65"/>
@@ -2858,38 +2894,40 @@
       <c r="M8" s="65"/>
       <c r="N8" s="29"/>
       <c r="P8" s="18" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
     </row>
     <row r="9" spans="1:16" s="12" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="21" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B9" s="38" t="s">
-        <v>206</v>
-      </c>
-      <c r="C9" s="46"/>
+        <v>204</v>
+      </c>
+      <c r="C9" s="38" t="s">
+        <v>204</v>
+      </c>
       <c r="D9" s="36" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="E9" s="39" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="F9" s="38" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="G9" s="38" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="H9" s="41"/>
       <c r="I9" s="45" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="J9" s="43" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="K9" s="42" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="L9" s="44"/>
       <c r="M9" s="44"/>
@@ -2900,33 +2938,35 @@
     </row>
     <row r="10" spans="1:16" s="12" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="21" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B10" s="38" t="s">
-        <v>206</v>
-      </c>
-      <c r="C10" s="46"/>
+        <v>204</v>
+      </c>
+      <c r="C10" s="38" t="s">
+        <v>204</v>
+      </c>
       <c r="D10" s="36" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="E10" s="39" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="F10" s="38" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="G10" s="38" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="H10" s="41"/>
       <c r="I10" s="45" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="J10" s="43" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="K10" s="42" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="L10" s="44"/>
       <c r="M10" s="44"/>
@@ -2935,33 +2975,35 @@
     </row>
     <row r="11" spans="1:16" s="12" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="21" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B11" s="38" t="s">
-        <v>206</v>
-      </c>
-      <c r="C11" s="46"/>
+        <v>204</v>
+      </c>
+      <c r="C11" s="38" t="s">
+        <v>204</v>
+      </c>
       <c r="D11" s="36" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="E11" s="39" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="F11" s="38" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="G11" s="38" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="H11" s="41"/>
       <c r="I11" s="45" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="J11" s="43" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="K11" s="42" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="L11" s="44"/>
       <c r="M11" s="44"/>
@@ -2970,190 +3012,200 @@
     </row>
     <row r="12" spans="1:16" s="12" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="21" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B12" s="38" t="s">
-        <v>206</v>
-      </c>
-      <c r="C12" s="46"/>
+        <v>204</v>
+      </c>
+      <c r="C12" s="38" t="s">
+        <v>204</v>
+      </c>
       <c r="D12" s="36" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="E12" s="39" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="F12" s="38" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="G12" s="38" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="H12" s="41"/>
       <c r="I12" s="45" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="J12" s="43" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="K12" s="42" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="L12" s="44"/>
       <c r="M12" s="44"/>
       <c r="N12" s="29"/>
       <c r="P12" s="13" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="13" spans="1:16" s="12" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="21" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B13" s="38" t="s">
-        <v>206</v>
-      </c>
-      <c r="C13" s="46"/>
+        <v>204</v>
+      </c>
+      <c r="C13" s="38" t="s">
+        <v>204</v>
+      </c>
       <c r="D13" s="36" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="E13" s="39" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="F13" s="38" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="G13" s="38" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="H13" s="41"/>
       <c r="I13" s="45" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="J13" s="43" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="K13" s="42" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="L13" s="44"/>
       <c r="M13" s="44"/>
       <c r="N13" s="29"/>
       <c r="P13" s="14" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="14" spans="1:16" s="12" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="21" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B14" s="38" t="s">
-        <v>206</v>
-      </c>
-      <c r="C14" s="46"/>
+        <v>204</v>
+      </c>
+      <c r="C14" s="38" t="s">
+        <v>204</v>
+      </c>
       <c r="D14" s="36" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="E14" s="39" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="F14" s="38" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="G14" s="38" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="H14" s="41"/>
       <c r="I14" s="45" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="J14" s="43" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="K14" s="42" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="L14" s="44"/>
       <c r="M14" s="44"/>
       <c r="N14" s="29"/>
       <c r="P14" s="14" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="15" spans="1:16" s="12" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B15" s="46"/>
-      <c r="C15" s="46"/>
+      <c r="C15" s="45" t="s">
+        <v>253</v>
+      </c>
       <c r="D15" s="47" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="E15" s="38" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="F15" s="38" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="G15" s="48" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="H15" s="41"/>
       <c r="I15" s="42" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="J15" s="42" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="K15" s="45" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="L15" s="44"/>
       <c r="M15" s="44"/>
       <c r="N15" s="29"/>
       <c r="P15" s="14" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="16" spans="1:16" s="12" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B16" s="49"/>
-      <c r="C16" s="49"/>
+      <c r="C16" s="45" t="s">
+        <v>253</v>
+      </c>
       <c r="D16" s="47" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="E16" s="37" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="F16" s="50" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="G16" s="36" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="H16" s="41"/>
       <c r="I16" s="45" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="J16" s="45" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="K16" s="45" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="L16" s="44"/>
       <c r="M16" s="44"/>
       <c r="N16" s="32" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="P16" s="14" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="17" spans="1:16" s="12" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="26" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B17" s="63"/>
       <c r="C17" s="63"/>
@@ -3162,7 +3214,7 @@
       <c r="F17" s="63"/>
       <c r="G17" s="63"/>
       <c r="H17" s="41" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="I17" s="65"/>
       <c r="J17" s="65"/>
@@ -3171,70 +3223,74 @@
       <c r="M17" s="65"/>
       <c r="N17" s="29"/>
       <c r="P17" s="15" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
     </row>
     <row r="18" spans="1:16" s="12" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="21" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B18" s="51"/>
-      <c r="C18" s="51"/>
+      <c r="C18" s="45" t="s">
+        <v>253</v>
+      </c>
       <c r="D18" s="47" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="E18" s="39" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="F18" s="39" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="G18" s="48" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="H18" s="41"/>
       <c r="I18" s="45" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="J18" s="52" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="K18" s="45" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="L18" s="44"/>
       <c r="M18" s="44"/>
       <c r="N18" s="62" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
     </row>
     <row r="19" spans="1:16" s="12" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="21" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B19" s="51"/>
-      <c r="C19" s="51"/>
+      <c r="C19" s="45" t="s">
+        <v>253</v>
+      </c>
       <c r="D19" s="47" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="E19" s="39" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="F19" s="39" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="G19" s="48" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="H19" s="41"/>
       <c r="I19" s="45" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="J19" s="52" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="K19" s="45" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="L19" s="44"/>
       <c r="M19" s="44"/>
@@ -3242,31 +3298,33 @@
     </row>
     <row r="20" spans="1:16" s="12" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="21" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B20" s="51"/>
-      <c r="C20" s="51"/>
+      <c r="C20" s="45" t="s">
+        <v>253</v>
+      </c>
       <c r="D20" s="47" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="E20" s="39" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="F20" s="39" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="G20" s="48" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="H20" s="41"/>
       <c r="I20" s="45" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="J20" s="52" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="K20" s="45" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="L20" s="44"/>
       <c r="M20" s="44"/>
@@ -3274,31 +3332,33 @@
     </row>
     <row r="21" spans="1:16" s="12" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="21" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B21" s="51"/>
-      <c r="C21" s="51"/>
+      <c r="C21" s="45" t="s">
+        <v>253</v>
+      </c>
       <c r="D21" s="47" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="E21" s="39" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="F21" s="39" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="G21" s="48" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="H21" s="41"/>
       <c r="I21" s="45" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="J21" s="52" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="K21" s="45" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="L21" s="44"/>
       <c r="M21" s="44"/>
@@ -3306,31 +3366,33 @@
     </row>
     <row r="22" spans="1:16" s="12" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="21" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B22" s="51"/>
-      <c r="C22" s="51"/>
+      <c r="C22" s="45" t="s">
+        <v>253</v>
+      </c>
       <c r="D22" s="47" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="E22" s="39" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="F22" s="39" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="G22" s="48" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="H22" s="41"/>
       <c r="I22" s="45" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="J22" s="52" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="K22" s="45" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="L22" s="44"/>
       <c r="M22" s="44"/>
@@ -3338,31 +3400,33 @@
     </row>
     <row r="23" spans="1:16" s="12" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="21" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B23" s="51"/>
-      <c r="C23" s="51"/>
+      <c r="C23" s="45" t="s">
+        <v>253</v>
+      </c>
       <c r="D23" s="47" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="E23" s="39" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="F23" s="39" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="G23" s="48" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="H23" s="41"/>
       <c r="I23" s="45" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="J23" s="52" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="K23" s="45" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="L23" s="44"/>
       <c r="M23" s="44"/>
@@ -3370,59 +3434,61 @@
     </row>
     <row r="24" spans="1:16" s="12" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="21" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B24" s="51"/>
       <c r="C24" s="51"/>
       <c r="D24" s="36" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="E24" s="38" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="F24" s="39" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="G24" s="51"/>
       <c r="H24" s="41" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="I24" s="42" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="J24" s="42" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="K24" s="43" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="L24" s="44"/>
       <c r="M24" s="44"/>
       <c r="N24" s="32" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="25" spans="1:16" s="12" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="21" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B25" s="51"/>
       <c r="C25" s="51"/>
       <c r="D25" s="36" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="E25" s="39" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="F25" s="38" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="G25" s="51"/>
       <c r="H25" s="41" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="I25" s="53"/>
-      <c r="J25" s="44"/>
+      <c r="J25" s="50" t="s">
+        <v>278</v>
+      </c>
       <c r="K25" s="44"/>
       <c r="L25" s="44"/>
       <c r="M25" s="44"/>
@@ -3430,67 +3496,69 @@
     </row>
     <row r="26" spans="1:16" s="12" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="21" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B26" s="51"/>
       <c r="C26" s="51"/>
       <c r="D26" s="36" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="E26" s="38" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="F26" s="38" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="G26" s="51"/>
       <c r="H26" s="41" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="I26" s="44" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="J26" s="44" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="K26" s="44" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="L26" s="44"/>
       <c r="M26" s="44"/>
       <c r="N26" s="32" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="27" spans="1:16" s="12" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="21" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B27" s="38" t="s">
-        <v>206</v>
-      </c>
-      <c r="C27" s="51"/>
+        <v>204</v>
+      </c>
+      <c r="C27" s="38" t="s">
+        <v>204</v>
+      </c>
       <c r="D27" s="38" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="E27" s="38" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="F27" s="38" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="G27" s="38" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="H27" s="41" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="I27" s="45" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="J27" s="53"/>
       <c r="K27" s="42" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="L27" s="44"/>
       <c r="M27" s="44"/>
@@ -3519,22 +3587,26 @@
         <v>182</v>
       </c>
       <c r="B29" s="54"/>
-      <c r="C29" s="54"/>
+      <c r="C29" s="47" t="s">
+        <v>235</v>
+      </c>
       <c r="D29" s="47" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="E29" s="37" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="F29" s="55" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="G29" s="48" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="H29" s="41"/>
       <c r="I29" s="53"/>
-      <c r="J29" s="44"/>
+      <c r="J29" s="45" t="s">
+        <v>278</v>
+      </c>
       <c r="K29" s="44"/>
       <c r="L29" s="44"/>
       <c r="M29" s="44"/>
@@ -3545,56 +3617,60 @@
         <v>184</v>
       </c>
       <c r="B30" s="54"/>
-      <c r="C30" s="54"/>
+      <c r="C30" s="68" t="s">
+        <v>235</v>
+      </c>
       <c r="D30" s="47" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="E30" s="37" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="F30" s="55" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="G30" s="48" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="H30" s="41"/>
       <c r="I30" s="52" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="J30" s="43" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="K30" s="43" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="L30" s="44"/>
       <c r="M30" s="44"/>
       <c r="N30" s="32" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B31" s="54"/>
       <c r="C31" s="54"/>
       <c r="D31" s="55" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="E31" s="48" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="F31" s="55" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="G31" s="48" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="H31" s="41"/>
       <c r="I31" s="53"/>
-      <c r="J31" s="40"/>
+      <c r="J31" s="38" t="s">
+        <v>278</v>
+      </c>
       <c r="K31" s="40"/>
       <c r="L31" s="40"/>
       <c r="M31" s="40"/>
@@ -3607,292 +3683,288 @@
       <c r="B32" s="54"/>
       <c r="C32" s="54"/>
       <c r="D32" s="55" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="E32" s="48" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="F32" s="55" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="G32" s="48" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="H32" s="41"/>
       <c r="I32" s="50" t="s">
-        <v>281</v>
-      </c>
-      <c r="J32" s="40"/>
+        <v>278</v>
+      </c>
+      <c r="J32" s="50" t="s">
+        <v>278</v>
+      </c>
       <c r="K32" s="40"/>
       <c r="L32" s="40"/>
       <c r="M32" s="40"/>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>187</v>
+        <v>237</v>
       </c>
       <c r="B33" s="54"/>
       <c r="C33" s="54"/>
       <c r="D33" s="55" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="E33" s="48" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="F33" s="55" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="G33" s="48" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="H33" s="41"/>
-      <c r="I33" s="51"/>
-      <c r="J33" s="40"/>
+      <c r="I33" s="25"/>
+      <c r="J33" s="39" t="s">
+        <v>278</v>
+      </c>
       <c r="K33" s="40"/>
       <c r="L33" s="40"/>
       <c r="M33" s="40"/>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B34" s="54"/>
       <c r="C34" s="54"/>
       <c r="D34" s="55" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="E34" s="48" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="F34" s="55" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="G34" s="48" t="s">
-        <v>237</v>
-      </c>
-      <c r="H34" s="41" t="s">
+        <v>235</v>
+      </c>
+      <c r="H34" s="41"/>
+      <c r="I34" s="50" t="s">
         <v>278</v>
       </c>
-      <c r="I34" s="25"/>
-      <c r="J34" s="40"/>
+      <c r="J34" s="39" t="s">
+        <v>278</v>
+      </c>
       <c r="K34" s="40"/>
       <c r="L34" s="40"/>
       <c r="M34" s="40"/>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>239</v>
+        <v>186</v>
       </c>
       <c r="B35" s="54"/>
       <c r="C35" s="54"/>
-      <c r="D35" s="55" t="s">
-        <v>237</v>
+      <c r="D35" s="48" t="s">
+        <v>235</v>
       </c>
       <c r="E35" s="48" t="s">
-        <v>237</v>
-      </c>
-      <c r="F35" s="55" t="s">
-        <v>237</v>
+        <v>235</v>
+      </c>
+      <c r="F35" s="48" t="s">
+        <v>235</v>
       </c>
       <c r="G35" s="48" t="s">
-        <v>237</v>
-      </c>
-      <c r="H35" s="41"/>
+        <v>235</v>
+      </c>
+      <c r="H35" s="41" t="s">
+        <v>276</v>
+      </c>
       <c r="I35" s="25"/>
-      <c r="J35" s="40"/>
+      <c r="J35" s="53"/>
       <c r="K35" s="40"/>
       <c r="L35" s="40"/>
       <c r="M35" s="40"/>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>189</v>
+        <v>241</v>
       </c>
       <c r="B36" s="54"/>
       <c r="C36" s="54"/>
       <c r="D36" s="55" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="E36" s="48" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="F36" s="55" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="G36" s="48" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="H36" s="41"/>
       <c r="I36" s="50" t="s">
-        <v>281</v>
-      </c>
-      <c r="J36" s="40"/>
+        <v>278</v>
+      </c>
+      <c r="J36" s="53"/>
       <c r="K36" s="40"/>
       <c r="L36" s="40"/>
       <c r="M36" s="40"/>
+      <c r="N36" s="31" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>186</v>
+        <v>10</v>
       </c>
       <c r="B37" s="54"/>
       <c r="C37" s="54"/>
-      <c r="D37" s="48" t="s">
-        <v>237</v>
+      <c r="D37" s="55" t="s">
+        <v>235</v>
       </c>
       <c r="E37" s="48" t="s">
-        <v>237</v>
-      </c>
-      <c r="F37" s="48" t="s">
-        <v>237</v>
+        <v>235</v>
+      </c>
+      <c r="F37" s="55" t="s">
+        <v>235</v>
       </c>
       <c r="G37" s="48" t="s">
-        <v>237</v>
-      </c>
-      <c r="H37" s="41" t="s">
-        <v>279</v>
-      </c>
+        <v>235</v>
+      </c>
+      <c r="H37" s="41"/>
       <c r="I37" s="25"/>
-      <c r="J37" s="40"/>
+      <c r="J37" s="39" t="s">
+        <v>278</v>
+      </c>
       <c r="K37" s="40"/>
       <c r="L37" s="40"/>
       <c r="M37" s="40"/>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>243</v>
+        <v>277</v>
       </c>
       <c r="B38" s="54"/>
       <c r="C38" s="54"/>
       <c r="D38" s="55" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="E38" s="48" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="F38" s="55" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="G38" s="48" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="H38" s="41"/>
-      <c r="I38" s="50" t="s">
-        <v>281</v>
-      </c>
-      <c r="J38" s="40"/>
-      <c r="K38" s="40"/>
+      <c r="I38" s="42" t="s">
+        <v>253</v>
+      </c>
+      <c r="J38" s="42" t="s">
+        <v>253</v>
+      </c>
+      <c r="K38" s="48" t="s">
+        <v>253</v>
+      </c>
       <c r="L38" s="40"/>
       <c r="M38" s="40"/>
       <c r="N38" s="31" t="s">
-        <v>289</v>
+        <v>267</v>
       </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>10</v>
-      </c>
-      <c r="B39" s="54"/>
+        <v>188</v>
+      </c>
+      <c r="B39" s="48" t="s">
+        <v>235</v>
+      </c>
       <c r="C39" s="54"/>
-      <c r="D39" s="55" t="s">
-        <v>237</v>
+      <c r="D39" s="48" t="s">
+        <v>235</v>
       </c>
       <c r="E39" s="48" t="s">
-        <v>237</v>
-      </c>
-      <c r="F39" s="55" t="s">
-        <v>237</v>
+        <v>278</v>
+      </c>
+      <c r="F39" s="48" t="s">
+        <v>235</v>
       </c>
       <c r="G39" s="48" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="H39" s="41"/>
-      <c r="I39" s="25"/>
-      <c r="J39" s="40"/>
+      <c r="I39" s="48" t="s">
+        <v>235</v>
+      </c>
+      <c r="J39" s="39" t="s">
+        <v>278</v>
+      </c>
       <c r="K39" s="40"/>
       <c r="L39" s="40"/>
       <c r="M39" s="40"/>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>280</v>
-      </c>
-      <c r="B40" s="54"/>
-      <c r="C40" s="54"/>
-      <c r="D40" s="55" t="s">
-        <v>237</v>
-      </c>
-      <c r="E40" s="48" t="s">
-        <v>237</v>
-      </c>
-      <c r="F40" s="55" t="s">
-        <v>237</v>
-      </c>
-      <c r="G40" s="48" t="s">
-        <v>237</v>
-      </c>
-      <c r="H40" s="41"/>
-      <c r="I40" s="42" t="s">
-        <v>255</v>
-      </c>
-      <c r="J40" s="42" t="s">
-        <v>255</v>
-      </c>
-      <c r="K40" s="48" t="s">
-        <v>255</v>
-      </c>
+        <v>238</v>
+      </c>
+      <c r="B40" s="56"/>
+      <c r="C40" s="56"/>
+      <c r="D40" s="56"/>
+      <c r="E40" s="40" t="s">
+        <v>284</v>
+      </c>
+      <c r="F40" s="56"/>
+      <c r="G40" s="40" t="s">
+        <v>279</v>
+      </c>
+      <c r="H40" s="41" t="s">
+        <v>239</v>
+      </c>
+      <c r="I40" s="40"/>
+      <c r="J40" s="40" t="s">
+        <v>279</v>
+      </c>
+      <c r="K40" s="40"/>
       <c r="L40" s="40"/>
       <c r="M40" s="40"/>
-      <c r="N40" s="31" t="s">
-        <v>269</v>
-      </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>190</v>
-      </c>
-      <c r="B41" s="48" t="s">
-        <v>237</v>
-      </c>
-      <c r="C41" s="54"/>
-      <c r="D41" s="48" t="s">
-        <v>237</v>
-      </c>
-      <c r="E41" s="48" t="s">
-        <v>281</v>
-      </c>
-      <c r="F41" s="48" t="s">
-        <v>237</v>
-      </c>
-      <c r="G41" s="48" t="s">
-        <v>237</v>
-      </c>
+      <c r="A41" s="27" t="s">
+        <v>240</v>
+      </c>
+      <c r="B41" s="49"/>
+      <c r="C41" s="49"/>
+      <c r="D41" s="49"/>
+      <c r="E41" s="49"/>
+      <c r="F41" s="49"/>
+      <c r="G41" s="49"/>
       <c r="H41" s="41"/>
-      <c r="I41" s="48" t="s">
-        <v>237</v>
-      </c>
-      <c r="J41" s="40"/>
+      <c r="I41" s="51"/>
+      <c r="J41" s="51"/>
       <c r="K41" s="40"/>
       <c r="L41" s="40"/>
       <c r="M41" s="40"/>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>240</v>
+      <c r="A42" s="27" t="s">
+        <v>243</v>
       </c>
       <c r="B42" s="56"/>
       <c r="C42" s="56"/>
       <c r="D42" s="56"/>
       <c r="E42" s="40" t="s">
-        <v>287</v>
+        <v>279</v>
       </c>
       <c r="F42" s="56"/>
-      <c r="G42" s="40" t="s">
-        <v>282</v>
-      </c>
-      <c r="H42" s="41" t="s">
-        <v>241</v>
-      </c>
+      <c r="G42" s="56"/>
+      <c r="H42" s="41"/>
       <c r="I42" s="40"/>
       <c r="J42" s="40"/>
       <c r="K42" s="40"/>
@@ -3908,290 +3980,294 @@
       <c r="D43" s="49"/>
       <c r="E43" s="49"/>
       <c r="F43" s="49"/>
-      <c r="G43" s="49"/>
+      <c r="G43" s="54"/>
       <c r="H43" s="41"/>
       <c r="I43" s="51"/>
-      <c r="J43" s="40"/>
+      <c r="J43" s="51"/>
       <c r="K43" s="40"/>
       <c r="L43" s="40"/>
       <c r="M43" s="40"/>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44" s="27" t="s">
-        <v>245</v>
-      </c>
-      <c r="B44" s="56"/>
-      <c r="C44" s="56"/>
-      <c r="D44" s="56"/>
-      <c r="E44" s="40" t="s">
-        <v>282</v>
-      </c>
-      <c r="F44" s="56"/>
-      <c r="G44" s="56"/>
+        <v>9</v>
+      </c>
+      <c r="B44" s="51"/>
+      <c r="C44" s="51"/>
+      <c r="D44" s="51"/>
+      <c r="E44" s="51"/>
+      <c r="F44" s="51"/>
+      <c r="G44" s="51"/>
       <c r="H44" s="41"/>
-      <c r="I44" s="68"/>
-      <c r="J44" s="40"/>
+      <c r="I44" s="51"/>
+      <c r="J44" s="51"/>
       <c r="K44" s="40"/>
       <c r="L44" s="40"/>
       <c r="M44" s="40"/>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" s="27" t="s">
-        <v>244</v>
-      </c>
-      <c r="B45" s="49"/>
-      <c r="C45" s="49"/>
-      <c r="D45" s="49"/>
-      <c r="E45" s="49"/>
-      <c r="F45" s="49"/>
-      <c r="G45" s="54"/>
+        <v>246</v>
+      </c>
+      <c r="B45" s="51"/>
+      <c r="C45" s="51"/>
+      <c r="D45" s="51"/>
+      <c r="E45" s="51"/>
+      <c r="F45" s="51"/>
+      <c r="G45" s="51"/>
       <c r="H45" s="41"/>
       <c r="I45" s="51"/>
-      <c r="J45" s="40"/>
+      <c r="J45" s="51"/>
       <c r="K45" s="40"/>
       <c r="L45" s="40"/>
       <c r="M45" s="40"/>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A46" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="B46" s="51"/>
-      <c r="C46" s="51"/>
-      <c r="D46" s="51"/>
-      <c r="E46" s="51"/>
-      <c r="F46" s="51"/>
-      <c r="G46" s="51"/>
+      <c r="A46" s="33" t="s">
+        <v>285</v>
+      </c>
+      <c r="B46" s="40"/>
+      <c r="C46" s="40"/>
+      <c r="D46" s="40"/>
+      <c r="E46" s="40"/>
+      <c r="F46" s="40"/>
+      <c r="G46" s="40"/>
       <c r="H46" s="41"/>
-      <c r="I46" s="51"/>
+      <c r="I46" s="40"/>
       <c r="J46" s="40"/>
       <c r="K46" s="40"/>
       <c r="L46" s="40"/>
       <c r="M46" s="40"/>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A47" s="27" t="s">
-        <v>248</v>
+      <c r="A47" t="s">
+        <v>193</v>
       </c>
       <c r="B47" s="51"/>
       <c r="C47" s="51"/>
-      <c r="D47" s="51"/>
-      <c r="E47" s="51"/>
+      <c r="D47" s="47" t="s">
+        <v>253</v>
+      </c>
+      <c r="E47" s="37" t="s">
+        <v>253</v>
+      </c>
       <c r="F47" s="51"/>
       <c r="G47" s="51"/>
-      <c r="H47" s="41"/>
-      <c r="I47" s="51"/>
-      <c r="J47" s="40"/>
-      <c r="K47" s="40"/>
-      <c r="L47" s="40"/>
+      <c r="H47" s="57"/>
+      <c r="I47" s="47" t="s">
+        <v>253</v>
+      </c>
+      <c r="J47" s="37" t="s">
+        <v>253</v>
+      </c>
+      <c r="K47" s="47" t="s">
+        <v>253</v>
+      </c>
+      <c r="L47" s="56"/>
       <c r="M47" s="40"/>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A48" s="33" t="s">
-        <v>288</v>
-      </c>
-      <c r="B48" s="68"/>
-      <c r="C48" s="68"/>
-      <c r="D48" s="68"/>
-      <c r="E48" s="68"/>
-      <c r="F48" s="68"/>
-      <c r="G48" s="68"/>
+      <c r="A48" t="s">
+        <v>194</v>
+      </c>
+      <c r="B48" s="51"/>
+      <c r="C48" s="51"/>
+      <c r="D48" s="48" t="s">
+        <v>253</v>
+      </c>
+      <c r="E48" s="48" t="s">
+        <v>253</v>
+      </c>
+      <c r="F48" s="51"/>
+      <c r="G48" s="51"/>
       <c r="H48" s="41"/>
-      <c r="I48" s="40"/>
-      <c r="J48" s="40"/>
-      <c r="K48" s="40"/>
+      <c r="I48" s="48" t="s">
+        <v>253</v>
+      </c>
+      <c r="J48" s="48" t="s">
+        <v>253</v>
+      </c>
+      <c r="K48" s="48" t="s">
+        <v>253</v>
+      </c>
       <c r="L48" s="40"/>
       <c r="M48" s="40"/>
+      <c r="N48" s="31" t="s">
+        <v>266</v>
+      </c>
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B49" s="51"/>
       <c r="C49" s="51"/>
-      <c r="D49" s="47" t="s">
-        <v>255</v>
+      <c r="D49" s="48" t="s">
+        <v>253</v>
       </c>
       <c r="E49" s="37" t="s">
-        <v>255</v>
-      </c>
-      <c r="F49" s="51"/>
+        <v>253</v>
+      </c>
+      <c r="F49" s="58" t="s">
+        <v>278</v>
+      </c>
       <c r="G49" s="51"/>
-      <c r="H49" s="57"/>
-      <c r="I49" s="47" t="s">
-        <v>255</v>
-      </c>
-      <c r="J49" s="37" t="s">
-        <v>255</v>
-      </c>
-      <c r="K49" s="47" t="s">
-        <v>255</v>
-      </c>
-      <c r="L49" s="56"/>
+      <c r="H49" s="41"/>
+      <c r="I49" s="51"/>
+      <c r="J49" s="55" t="s">
+        <v>253</v>
+      </c>
+      <c r="K49" s="48" t="s">
+        <v>253</v>
+      </c>
+      <c r="L49" s="40"/>
       <c r="M49" s="40"/>
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>196</v>
+        <v>268</v>
       </c>
       <c r="B50" s="51"/>
       <c r="C50" s="51"/>
       <c r="D50" s="48" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="E50" s="48" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="F50" s="51"/>
       <c r="G50" s="51"/>
       <c r="H50" s="41"/>
       <c r="I50" s="48" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="J50" s="48" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="K50" s="48" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="L50" s="40"/>
       <c r="M50" s="40"/>
-      <c r="N50" s="31" t="s">
-        <v>268</v>
-      </c>
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="B51" s="51"/>
       <c r="C51" s="51"/>
-      <c r="D51" s="48" t="s">
-        <v>255</v>
+      <c r="D51" s="47" t="s">
+        <v>253</v>
       </c>
       <c r="E51" s="37" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="F51" s="58" t="s">
-        <v>281</v>
-      </c>
-      <c r="G51" s="51"/>
+        <v>278</v>
+      </c>
+      <c r="G51" s="47" t="s">
+        <v>278</v>
+      </c>
       <c r="H51" s="41"/>
-      <c r="I51" s="51"/>
-      <c r="J51" s="55" t="s">
-        <v>255</v>
-      </c>
-      <c r="K51" s="48" t="s">
-        <v>255</v>
-      </c>
-      <c r="L51" s="40"/>
-      <c r="M51" s="40"/>
+      <c r="I51" s="47" t="s">
+        <v>253</v>
+      </c>
+      <c r="J51" s="37" t="s">
+        <v>253</v>
+      </c>
+      <c r="K51" s="37" t="s">
+        <v>253</v>
+      </c>
+      <c r="L51" s="56"/>
+      <c r="M51" s="56"/>
+      <c r="N51" s="23"/>
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="B52" s="51"/>
       <c r="C52" s="51"/>
       <c r="D52" s="48" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="E52" s="48" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="F52" s="51"/>
       <c r="G52" s="51"/>
       <c r="H52" s="41"/>
       <c r="I52" s="48" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="J52" s="48" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="K52" s="48" t="s">
-        <v>255</v>
-      </c>
-      <c r="L52" s="40"/>
-      <c r="M52" s="40"/>
+        <v>253</v>
+      </c>
+      <c r="L52" s="56"/>
+      <c r="M52" s="56"/>
+      <c r="N52" s="23"/>
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>203</v>
-      </c>
-      <c r="B53" s="51"/>
-      <c r="C53" s="51"/>
-      <c r="D53" s="47" t="s">
-        <v>255</v>
-      </c>
-      <c r="E53" s="37" t="s">
-        <v>255</v>
-      </c>
-      <c r="F53" s="58" t="s">
-        <v>281</v>
-      </c>
-      <c r="G53" s="47" t="s">
-        <v>281</v>
-      </c>
-      <c r="H53" s="41"/>
-      <c r="I53" s="47" t="s">
-        <v>255</v>
-      </c>
-      <c r="J53" s="37" t="s">
-        <v>255</v>
-      </c>
-      <c r="K53" s="37" t="s">
-        <v>255</v>
-      </c>
-      <c r="L53" s="56"/>
-      <c r="M53" s="56"/>
-      <c r="N53" s="23"/>
+      <c r="A53" s="28" t="s">
+        <v>263</v>
+      </c>
+      <c r="B53" s="67"/>
+      <c r="C53" s="67"/>
+      <c r="D53" s="67"/>
+      <c r="E53" s="67"/>
+      <c r="F53" s="67"/>
+      <c r="G53" s="67"/>
+      <c r="H53" s="23" t="s">
+        <v>264</v>
+      </c>
+      <c r="I53" s="67"/>
+      <c r="J53" s="67"/>
+      <c r="K53" s="67"/>
+      <c r="L53" s="67"/>
+      <c r="M53" s="67"/>
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>267</v>
-      </c>
-      <c r="B54" s="51"/>
-      <c r="C54" s="51"/>
-      <c r="D54" s="48" t="s">
-        <v>255</v>
-      </c>
-      <c r="E54" s="48" t="s">
-        <v>255</v>
-      </c>
-      <c r="F54" s="51"/>
-      <c r="G54" s="51"/>
-      <c r="H54" s="41"/>
-      <c r="I54" s="48" t="s">
-        <v>255</v>
-      </c>
-      <c r="J54" s="48" t="s">
-        <v>255</v>
-      </c>
-      <c r="K54" s="48" t="s">
-        <v>255</v>
-      </c>
-      <c r="L54" s="56"/>
-      <c r="M54" s="56"/>
-      <c r="N54" s="23"/>
+        <v>195</v>
+      </c>
+      <c r="B54" s="34"/>
+      <c r="C54" s="34"/>
+      <c r="D54" s="34"/>
+      <c r="E54" s="34"/>
+      <c r="F54" s="34"/>
+      <c r="G54" s="34"/>
+      <c r="H54" s="60" t="s">
+        <v>269</v>
+      </c>
+      <c r="I54" s="34"/>
+      <c r="J54" s="35"/>
+      <c r="K54" s="34"/>
+      <c r="L54" s="35"/>
+      <c r="M54" s="25"/>
+      <c r="N54" s="60" t="s">
+        <v>269</v>
+      </c>
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A55" s="28" t="s">
-        <v>265</v>
-      </c>
-      <c r="B55" s="67"/>
-      <c r="C55" s="67"/>
-      <c r="D55" s="67"/>
-      <c r="E55" s="67"/>
-      <c r="F55" s="67"/>
-      <c r="G55" s="67"/>
-      <c r="H55" s="23" t="s">
-        <v>266</v>
-      </c>
-      <c r="I55" s="67"/>
-      <c r="J55" s="67"/>
-      <c r="K55" s="67"/>
-      <c r="L55" s="67"/>
-      <c r="M55" s="67"/>
+      <c r="A55" t="s">
+        <v>192</v>
+      </c>
+      <c r="B55" s="34"/>
+      <c r="C55" s="34"/>
+      <c r="D55" s="34"/>
+      <c r="E55" s="34"/>
+      <c r="F55" s="34"/>
+      <c r="G55" s="34"/>
+      <c r="H55" s="60"/>
+      <c r="I55" s="35"/>
+      <c r="J55" s="35"/>
+      <c r="K55" s="35"/>
+      <c r="L55" s="35"/>
+      <c r="M55" s="25"/>
+      <c r="N55" s="60"/>
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
@@ -4203,21 +4279,17 @@
       <c r="E56" s="34"/>
       <c r="F56" s="34"/>
       <c r="G56" s="34"/>
-      <c r="H56" s="60" t="s">
-        <v>271</v>
-      </c>
-      <c r="I56" s="34"/>
+      <c r="H56" s="60"/>
+      <c r="I56" s="35"/>
       <c r="J56" s="35"/>
-      <c r="K56" s="34"/>
+      <c r="K56" s="35"/>
       <c r="L56" s="35"/>
       <c r="M56" s="25"/>
-      <c r="N56" s="60" t="s">
-        <v>271</v>
-      </c>
+      <c r="N56" s="60"/>
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="B57" s="34"/>
       <c r="C57" s="34"/>
@@ -4226,11 +4298,11 @@
       <c r="F57" s="34"/>
       <c r="G57" s="34"/>
       <c r="H57" s="60"/>
-      <c r="I57" s="35"/>
-      <c r="J57" s="35"/>
-      <c r="K57" s="35"/>
-      <c r="L57" s="35"/>
-      <c r="M57" s="25"/>
+      <c r="I57" s="34"/>
+      <c r="J57" s="34"/>
+      <c r="K57" s="34"/>
+      <c r="L57" s="34"/>
+      <c r="M57" s="24"/>
       <c r="N57" s="60"/>
     </row>
     <row r="58" spans="1:14" x14ac:dyDescent="0.25">
@@ -4244,11 +4316,11 @@
       <c r="F58" s="34"/>
       <c r="G58" s="34"/>
       <c r="H58" s="60"/>
-      <c r="I58" s="35"/>
-      <c r="J58" s="35"/>
-      <c r="K58" s="35"/>
-      <c r="L58" s="35"/>
-      <c r="M58" s="25"/>
+      <c r="I58" s="34"/>
+      <c r="J58" s="34"/>
+      <c r="K58" s="34"/>
+      <c r="L58" s="34"/>
+      <c r="M58" s="24"/>
       <c r="N58" s="60"/>
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.25">
@@ -4270,80 +4342,76 @@
       <c r="N59" s="60"/>
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>201</v>
-      </c>
-      <c r="B60" s="34"/>
-      <c r="C60" s="34"/>
-      <c r="D60" s="34"/>
-      <c r="E60" s="34"/>
-      <c r="F60" s="34"/>
-      <c r="G60" s="34"/>
-      <c r="H60" s="60"/>
-      <c r="I60" s="34"/>
-      <c r="J60" s="34"/>
-      <c r="K60" s="34"/>
-      <c r="L60" s="34"/>
-      <c r="M60" s="24"/>
-      <c r="N60" s="60"/>
+      <c r="A60" s="28" t="s">
+        <v>244</v>
+      </c>
+      <c r="B60" s="67"/>
+      <c r="C60" s="67"/>
+      <c r="D60" s="67"/>
+      <c r="E60" s="67"/>
+      <c r="F60" s="67"/>
+      <c r="G60" s="67"/>
+      <c r="I60" s="67"/>
+      <c r="J60" s="67"/>
+      <c r="K60" s="67"/>
+      <c r="L60" s="67"/>
+      <c r="M60" s="67"/>
     </row>
     <row r="61" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>202</v>
-      </c>
-      <c r="B61" s="34"/>
-      <c r="C61" s="34"/>
-      <c r="D61" s="34"/>
-      <c r="E61" s="34"/>
-      <c r="F61" s="34"/>
-      <c r="G61" s="34"/>
-      <c r="H61" s="60"/>
-      <c r="I61" s="34"/>
-      <c r="J61" s="34"/>
-      <c r="K61" s="34"/>
-      <c r="L61" s="34"/>
-      <c r="M61" s="24"/>
-      <c r="N61" s="60"/>
+        <v>247</v>
+      </c>
+      <c r="B61" s="64" t="s">
+        <v>260</v>
+      </c>
+      <c r="C61" s="64"/>
+      <c r="D61" s="64"/>
+      <c r="E61" s="64"/>
+      <c r="F61" s="64"/>
+      <c r="G61" s="64"/>
+      <c r="I61" s="64" t="s">
+        <v>260</v>
+      </c>
+      <c r="J61" s="64"/>
+      <c r="K61" s="64"/>
+      <c r="L61" s="64"/>
+      <c r="M61" s="64"/>
     </row>
     <row r="62" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A62" s="28" t="s">
-        <v>246</v>
-      </c>
-      <c r="B62" s="67"/>
-      <c r="C62" s="67"/>
-      <c r="D62" s="67"/>
-      <c r="E62" s="67"/>
-      <c r="F62" s="67"/>
-      <c r="G62" s="67"/>
-      <c r="I62" s="67"/>
-      <c r="J62" s="67"/>
-      <c r="K62" s="67"/>
-      <c r="L62" s="67"/>
-      <c r="M62" s="67"/>
+      <c r="A62" t="s">
+        <v>248</v>
+      </c>
+      <c r="B62" s="64"/>
+      <c r="C62" s="64"/>
+      <c r="D62" s="64"/>
+      <c r="E62" s="64"/>
+      <c r="F62" s="64"/>
+      <c r="G62" s="64"/>
+      <c r="I62" s="64"/>
+      <c r="J62" s="64"/>
+      <c r="K62" s="64"/>
+      <c r="L62" s="64"/>
+      <c r="M62" s="64"/>
     </row>
     <row r="63" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>249</v>
-      </c>
-      <c r="B63" s="64" t="s">
-        <v>262</v>
-      </c>
+        <v>176</v>
+      </c>
+      <c r="B63" s="64"/>
       <c r="C63" s="64"/>
       <c r="D63" s="64"/>
       <c r="E63" s="64"/>
       <c r="F63" s="64"/>
       <c r="G63" s="64"/>
-      <c r="I63" s="64" t="s">
-        <v>262</v>
-      </c>
+      <c r="I63" s="64"/>
       <c r="J63" s="64"/>
       <c r="K63" s="64"/>
       <c r="L63" s="64"/>
       <c r="M63" s="64"/>
     </row>
     <row r="64" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>250</v>
+      <c r="A64" s="12" t="s">
+        <v>189</v>
       </c>
       <c r="B64" s="64"/>
       <c r="C64" s="64"/>
@@ -4359,7 +4427,7 @@
     </row>
     <row r="65" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>176</v>
+        <v>249</v>
       </c>
       <c r="B65" s="64"/>
       <c r="C65" s="64"/>
@@ -4374,8 +4442,8 @@
       <c r="M65" s="64"/>
     </row>
     <row r="66" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A66" s="12" t="s">
-        <v>191</v>
+      <c r="A66" t="s">
+        <v>252</v>
       </c>
       <c r="B66" s="64"/>
       <c r="C66" s="64"/>
@@ -4391,7 +4459,7 @@
     </row>
     <row r="67" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>251</v>
+        <v>289</v>
       </c>
       <c r="B67" s="64"/>
       <c r="C67" s="64"/>
@@ -4407,7 +4475,7 @@
     </row>
     <row r="68" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="B68" s="64"/>
       <c r="C68" s="64"/>
@@ -4422,52 +4490,52 @@
       <c r="M68" s="64"/>
     </row>
     <row r="69" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
-        <v>253</v>
-      </c>
-      <c r="B69" s="64"/>
-      <c r="C69" s="64"/>
-      <c r="D69" s="64"/>
-      <c r="E69" s="64"/>
-      <c r="F69" s="64"/>
-      <c r="G69" s="64"/>
-      <c r="I69" s="64"/>
-      <c r="J69" s="64"/>
-      <c r="K69" s="64"/>
-      <c r="L69" s="64"/>
-      <c r="M69" s="64"/>
+      <c r="A69" s="28" t="s">
+        <v>245</v>
+      </c>
+      <c r="B69" s="67"/>
+      <c r="C69" s="67"/>
+      <c r="D69" s="67"/>
+      <c r="E69" s="67"/>
+      <c r="F69" s="67"/>
+      <c r="G69" s="67"/>
+      <c r="I69" s="67"/>
+      <c r="J69" s="67"/>
+      <c r="K69" s="67"/>
+      <c r="L69" s="67"/>
+      <c r="M69" s="67"/>
     </row>
     <row r="70" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A70" s="28" t="s">
-        <v>247</v>
-      </c>
-      <c r="B70" s="67"/>
-      <c r="C70" s="67"/>
-      <c r="D70" s="67"/>
-      <c r="E70" s="67"/>
-      <c r="F70" s="67"/>
-      <c r="G70" s="67"/>
-      <c r="I70" s="67"/>
-      <c r="J70" s="67"/>
-      <c r="K70" s="67"/>
-      <c r="L70" s="67"/>
-      <c r="M70" s="67"/>
+      <c r="A70" t="s">
+        <v>250</v>
+      </c>
+      <c r="B70" s="66" t="s">
+        <v>270</v>
+      </c>
+      <c r="C70" s="66"/>
+      <c r="D70" s="66"/>
+      <c r="E70" s="66"/>
+      <c r="F70" s="66"/>
+      <c r="G70" s="66"/>
+      <c r="I70" s="66" t="s">
+        <v>270</v>
+      </c>
+      <c r="J70" s="66"/>
+      <c r="K70" s="66"/>
+      <c r="L70" s="66"/>
+      <c r="M70" s="66"/>
     </row>
     <row r="71" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>252</v>
-      </c>
-      <c r="B71" s="66" t="s">
-        <v>272</v>
-      </c>
+        <v>261</v>
+      </c>
+      <c r="B71" s="66"/>
       <c r="C71" s="66"/>
       <c r="D71" s="66"/>
       <c r="E71" s="66"/>
       <c r="F71" s="66"/>
       <c r="G71" s="66"/>
-      <c r="I71" s="66" t="s">
-        <v>272</v>
-      </c>
+      <c r="I71" s="66"/>
       <c r="J71" s="66"/>
       <c r="K71" s="66"/>
       <c r="L71" s="66"/>
@@ -4475,7 +4543,7 @@
     </row>
     <row r="72" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B72" s="66"/>
       <c r="C72" s="66"/>
@@ -4490,20 +4558,19 @@
       <c r="M72" s="66"/>
     </row>
     <row r="73" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
-        <v>264</v>
-      </c>
-      <c r="B73" s="66"/>
-      <c r="C73" s="66"/>
-      <c r="D73" s="66"/>
-      <c r="E73" s="66"/>
-      <c r="F73" s="66"/>
-      <c r="G73" s="66"/>
-      <c r="I73" s="66"/>
-      <c r="J73" s="66"/>
-      <c r="K73" s="66"/>
-      <c r="L73" s="66"/>
-      <c r="M73" s="66"/>
+      <c r="B73" s="1"/>
+      <c r="C73" s="1"/>
+      <c r="D73" s="1"/>
+      <c r="E73" s="1"/>
+      <c r="F73" s="1"/>
+      <c r="G73" s="1"/>
+      <c r="H73" s="33"/>
+      <c r="I73" s="1"/>
+      <c r="J73" s="1"/>
+      <c r="K73" s="1"/>
+      <c r="L73" s="1"/>
+      <c r="M73" s="1"/>
+      <c r="N73"/>
     </row>
     <row r="74" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B74" s="1"/>
@@ -4566,6 +4633,7 @@
       <c r="N77"/>
     </row>
     <row r="78" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A78" s="12"/>
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
       <c r="D78" s="1"/>
@@ -4613,13 +4681,6 @@
       <c r="N80"/>
     </row>
     <row r="81" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A81" s="12"/>
-      <c r="B81" s="1"/>
-      <c r="C81" s="1"/>
-      <c r="D81" s="1"/>
-      <c r="E81" s="1"/>
-      <c r="F81" s="1"/>
-      <c r="G81" s="1"/>
       <c r="H81" s="33"/>
       <c r="I81" s="1"/>
       <c r="J81" s="1"/>
@@ -4665,6 +4726,13 @@
       <c r="N85"/>
     </row>
     <row r="86" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A86" s="12"/>
+      <c r="B86" s="1"/>
+      <c r="C86" s="1"/>
+      <c r="D86" s="1"/>
+      <c r="E86" s="1"/>
+      <c r="F86" s="1"/>
+      <c r="G86" s="1"/>
       <c r="H86" s="33"/>
       <c r="I86" s="1"/>
       <c r="J86" s="1"/>
@@ -5826,19 +5894,7 @@
       <c r="N158"/>
     </row>
     <row r="159" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A159" s="12"/>
-      <c r="B159" s="1"/>
-      <c r="C159" s="1"/>
-      <c r="D159" s="1"/>
-      <c r="E159" s="1"/>
-      <c r="F159" s="1"/>
-      <c r="G159" s="1"/>
       <c r="H159" s="33"/>
-      <c r="I159" s="1"/>
-      <c r="J159" s="1"/>
-      <c r="K159" s="1"/>
-      <c r="L159" s="1"/>
-      <c r="M159" s="1"/>
       <c r="N159"/>
     </row>
     <row r="160" spans="1:14" x14ac:dyDescent="0.25">
@@ -12413,27 +12469,23 @@
       <c r="H1802" s="33"/>
       <c r="N1802"/>
     </row>
-    <row r="1803" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H1803" s="33"/>
-      <c r="N1803"/>
-    </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="B63:G69"/>
+    <mergeCell ref="B61:G68"/>
     <mergeCell ref="I17:M17"/>
     <mergeCell ref="I8:M8"/>
-    <mergeCell ref="B71:G73"/>
-    <mergeCell ref="B55:G55"/>
-    <mergeCell ref="B62:G62"/>
-    <mergeCell ref="I55:M55"/>
-    <mergeCell ref="I70:M70"/>
-    <mergeCell ref="I63:M69"/>
-    <mergeCell ref="I71:M73"/>
-    <mergeCell ref="H56:H61"/>
-    <mergeCell ref="I62:M62"/>
-    <mergeCell ref="B70:G70"/>
+    <mergeCell ref="B70:G72"/>
+    <mergeCell ref="B53:G53"/>
+    <mergeCell ref="B60:G60"/>
+    <mergeCell ref="I53:M53"/>
+    <mergeCell ref="I69:M69"/>
+    <mergeCell ref="I61:M68"/>
+    <mergeCell ref="I70:M72"/>
+    <mergeCell ref="H54:H59"/>
+    <mergeCell ref="I60:M60"/>
+    <mergeCell ref="B69:G69"/>
     <mergeCell ref="I28:M28"/>
-    <mergeCell ref="N56:N61"/>
+    <mergeCell ref="N54:N59"/>
     <mergeCell ref="B28:G28"/>
     <mergeCell ref="N18:N23"/>
     <mergeCell ref="B8:G8"/>

</xml_diff>